<commit_message>
added support modal  bootstrap
</commit_message>
<xml_diff>
--- a/storage/download.xlsx
+++ b/storage/download.xlsx
@@ -143,7 +143,7 @@
         </is>
       </c>
       <c r="G2" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" s="0" t="inlineStr">
         <is>
@@ -291,7 +291,7 @@
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>Salmão a Fiorentina</t>
+          <t>Salmão a Fiorentina 2</t>
         </is>
       </c>
       <c r="C6" s="0" t="inlineStr">
@@ -1089,7 +1089,7 @@
         </is>
       </c>
       <c r="G24" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="0" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
main - add properties model
</commit_message>
<xml_diff>
--- a/storage/download.xlsx
+++ b/storage/download.xlsx
@@ -119,7 +119,7 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Pastel de Nata 2</t>
+          <t>Pastel de Nata</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
@@ -129,17 +129,17 @@
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>R$ 159,19</t>
+          <t>R$ 128,12</t>
         </is>
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>R$ 183,07</t>
+          <t>R$ 147,34</t>
         </is>
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t>720 kcal</t>
+          <t>286 kcal</t>
         </is>
       </c>
       <c r="G2" s="0">
@@ -147,12 +147,12 @@
       </c>
       <c r="H2" s="0" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="I2" s="0" t="inlineStr">
         <is>
-          <t>20/05/2021</t>
+          <t>25/06/2021</t>
         </is>
       </c>
     </row>
@@ -172,17 +172,17 @@
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>R$ 129,20</t>
+          <t>R$ 83,69</t>
         </is>
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>R$ 148,58</t>
+          <t>R$ 96,24</t>
         </is>
       </c>
       <c r="F3" s="0" t="inlineStr">
         <is>
-          <t>422 kcal</t>
+          <t>82 kcal</t>
         </is>
       </c>
       <c r="G3" s="0">
@@ -190,12 +190,12 @@
       </c>
       <c r="H3" s="0" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I3" s="0" t="inlineStr">
         <is>
-          <t>21/05/2021</t>
+          <t>13/07/2021</t>
         </is>
       </c>
     </row>
@@ -215,30 +215,30 @@
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>R$ 84,57</t>
+          <t>R$ 100,60</t>
         </is>
       </c>
       <c r="E4" s="0" t="inlineStr">
         <is>
-          <t>R$ 97,26</t>
+          <t>R$ 115,69</t>
         </is>
       </c>
       <c r="F4" s="0" t="inlineStr">
         <is>
-          <t>487 kcal</t>
+          <t>497 kcal</t>
         </is>
       </c>
       <c r="G4" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="0" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I4" s="0" t="inlineStr">
         <is>
-          <t>30/04/2021</t>
+          <t>23/06/2021</t>
         </is>
       </c>
     </row>
@@ -258,30 +258,30 @@
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>R$ 108,56</t>
+          <t>R$ 78,36</t>
         </is>
       </c>
       <c r="E5" s="0" t="inlineStr">
         <is>
-          <t>R$ 124,84</t>
+          <t>R$ 90,11</t>
         </is>
       </c>
       <c r="F5" s="0" t="inlineStr">
         <is>
-          <t>520 kcal</t>
+          <t>602 kcal</t>
         </is>
       </c>
       <c r="G5" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I5" s="0" t="inlineStr">
         <is>
-          <t>02/05/2021</t>
+          <t>27/06/2021</t>
         </is>
       </c>
     </row>
@@ -291,7 +291,7 @@
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>Salmão a Fiorentina 2</t>
+          <t>Salmão a Fiorentina</t>
         </is>
       </c>
       <c r="C6" s="0" t="inlineStr">
@@ -301,21 +301,21 @@
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>R$ 68,62</t>
+          <t>R$ 123,41</t>
         </is>
       </c>
       <c r="E6" s="0" t="inlineStr">
         <is>
-          <t>R$ 78,91</t>
+          <t>R$ 141,92</t>
         </is>
       </c>
       <c r="F6" s="0" t="inlineStr">
         <is>
-          <t>774 kcal</t>
+          <t>361 kcal</t>
         </is>
       </c>
       <c r="G6" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="0" t="inlineStr">
         <is>
@@ -324,7 +324,7 @@
       </c>
       <c r="I6" s="0" t="inlineStr">
         <is>
-          <t>09/05/2021</t>
+          <t>17/06/2021</t>
         </is>
       </c>
     </row>
@@ -344,30 +344,30 @@
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>R$ 94,75</t>
+          <t>R$ 84,17</t>
         </is>
       </c>
       <c r="E7" s="0" t="inlineStr">
         <is>
-          <t>R$ 108,96</t>
+          <t>R$ 96,80</t>
         </is>
       </c>
       <c r="F7" s="0" t="inlineStr">
         <is>
-          <t>674 kcal</t>
+          <t>566 kcal</t>
         </is>
       </c>
       <c r="G7" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="0" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="I7" s="0" t="inlineStr">
         <is>
-          <t>24/04/2021</t>
+          <t>06/07/2021</t>
         </is>
       </c>
     </row>
@@ -387,17 +387,17 @@
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>R$ 67,83</t>
+          <t>R$ 147,79</t>
         </is>
       </c>
       <c r="E8" s="0" t="inlineStr">
         <is>
-          <t>R$ 78,00</t>
+          <t>R$ 169,96</t>
         </is>
       </c>
       <c r="F8" s="0" t="inlineStr">
         <is>
-          <t>805 kcal</t>
+          <t>702 kcal</t>
         </is>
       </c>
       <c r="G8" s="0">
@@ -405,12 +405,12 @@
       </c>
       <c r="H8" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I8" s="0" t="inlineStr">
         <is>
-          <t>10/05/2021</t>
+          <t>14/07/2021</t>
         </is>
       </c>
     </row>
@@ -430,17 +430,17 @@
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>R$ 196,64</t>
+          <t>R$ 113,48</t>
         </is>
       </c>
       <c r="E9" s="0" t="inlineStr">
         <is>
-          <t>R$ 226,14</t>
+          <t>R$ 130,50</t>
         </is>
       </c>
       <c r="F9" s="0" t="inlineStr">
         <is>
-          <t>855 kcal</t>
+          <t>719 kcal</t>
         </is>
       </c>
       <c r="G9" s="0">
@@ -448,12 +448,12 @@
       </c>
       <c r="H9" s="0" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I9" s="0" t="inlineStr">
         <is>
-          <t>16/05/2021</t>
+          <t>05/07/2021</t>
         </is>
       </c>
     </row>
@@ -473,17 +473,17 @@
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>R$ 151,29</t>
+          <t>R$ 168,50</t>
         </is>
       </c>
       <c r="E10" s="0" t="inlineStr">
         <is>
-          <t>R$ 173,98</t>
+          <t>R$ 193,78</t>
         </is>
       </c>
       <c r="F10" s="0" t="inlineStr">
         <is>
-          <t>826 kcal</t>
+          <t>818 kcal</t>
         </is>
       </c>
       <c r="G10" s="0">
@@ -496,7 +496,7 @@
       </c>
       <c r="I10" s="0" t="inlineStr">
         <is>
-          <t>19/05/2021</t>
+          <t>04/07/2021</t>
         </is>
       </c>
     </row>
@@ -516,17 +516,17 @@
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>R$ 198,47</t>
+          <t>R$ 185,13</t>
         </is>
       </c>
       <c r="E11" s="0" t="inlineStr">
         <is>
-          <t>R$ 228,24</t>
+          <t>R$ 212,90</t>
         </is>
       </c>
       <c r="F11" s="0" t="inlineStr">
         <is>
-          <t>744 kcal</t>
+          <t>666 kcal</t>
         </is>
       </c>
       <c r="G11" s="0">
@@ -534,12 +534,12 @@
       </c>
       <c r="H11" s="0" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="I11" s="0" t="inlineStr">
         <is>
-          <t>26/04/2021</t>
+          <t>22/06/2021</t>
         </is>
       </c>
     </row>
@@ -559,30 +559,30 @@
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t>R$ 138,97</t>
+          <t>R$ 69,91</t>
         </is>
       </c>
       <c r="E12" s="0" t="inlineStr">
         <is>
-          <t>R$ 159,82</t>
+          <t>R$ 80,40</t>
         </is>
       </c>
       <c r="F12" s="0" t="inlineStr">
         <is>
-          <t>620 kcal</t>
+          <t>787 kcal</t>
         </is>
       </c>
       <c r="G12" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="0" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I12" s="0" t="inlineStr">
         <is>
-          <t>26/04/2021</t>
+          <t>26/06/2021</t>
         </is>
       </c>
     </row>
@@ -602,17 +602,17 @@
       </c>
       <c r="D13" s="0" t="inlineStr">
         <is>
-          <t>R$ 67,01</t>
+          <t>R$ 88,82</t>
         </is>
       </c>
       <c r="E13" s="0" t="inlineStr">
         <is>
-          <t>R$ 77,06</t>
+          <t>R$ 102,14</t>
         </is>
       </c>
       <c r="F13" s="0" t="inlineStr">
         <is>
-          <t>671 kcal</t>
+          <t>754 kcal</t>
         </is>
       </c>
       <c r="G13" s="0">
@@ -620,12 +620,12 @@
       </c>
       <c r="H13" s="0" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="I13" s="0" t="inlineStr">
         <is>
-          <t>12/05/2021</t>
+          <t>24/06/2021</t>
         </is>
       </c>
     </row>
@@ -645,17 +645,17 @@
       </c>
       <c r="D14" s="0" t="inlineStr">
         <is>
-          <t>R$ 119,18</t>
+          <t>R$ 103,58</t>
         </is>
       </c>
       <c r="E14" s="0" t="inlineStr">
         <is>
-          <t>R$ 137,06</t>
+          <t>R$ 119,12</t>
         </is>
       </c>
       <c r="F14" s="0" t="inlineStr">
         <is>
-          <t>566 kcal</t>
+          <t>684 kcal</t>
         </is>
       </c>
       <c r="G14" s="0">
@@ -668,7 +668,7 @@
       </c>
       <c r="I14" s="0" t="inlineStr">
         <is>
-          <t>26/04/2021</t>
+          <t>28/06/2021</t>
         </is>
       </c>
     </row>
@@ -688,30 +688,30 @@
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
-          <t>R$ 140,46</t>
+          <t>R$ 195,56</t>
         </is>
       </c>
       <c r="E15" s="0" t="inlineStr">
         <is>
-          <t>R$ 161,53</t>
+          <t>R$ 224,89</t>
         </is>
       </c>
       <c r="F15" s="0" t="inlineStr">
         <is>
-          <t>794 kcal</t>
+          <t>609 kcal</t>
         </is>
       </c>
       <c r="G15" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I15" s="0" t="inlineStr">
         <is>
-          <t>20/05/2021</t>
+          <t>02/07/2021</t>
         </is>
       </c>
     </row>
@@ -731,17 +731,17 @@
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
-          <t>R$ 171,32</t>
+          <t>R$ 186,45</t>
         </is>
       </c>
       <c r="E16" s="0" t="inlineStr">
         <is>
-          <t>R$ 197,02</t>
+          <t>R$ 214,42</t>
         </is>
       </c>
       <c r="F16" s="0" t="inlineStr">
         <is>
-          <t>640 kcal</t>
+          <t>413 kcal</t>
         </is>
       </c>
       <c r="G16" s="0">
@@ -749,12 +749,12 @@
       </c>
       <c r="H16" s="0" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="I16" s="0" t="inlineStr">
         <is>
-          <t>14/05/2021</t>
+          <t>27/06/2021</t>
         </is>
       </c>
     </row>
@@ -774,17 +774,17 @@
       </c>
       <c r="D17" s="0" t="inlineStr">
         <is>
-          <t>R$ 178,45</t>
+          <t>R$ 133,08</t>
         </is>
       </c>
       <c r="E17" s="0" t="inlineStr">
         <is>
-          <t>R$ 205,22</t>
+          <t>R$ 153,04</t>
         </is>
       </c>
       <c r="F17" s="0" t="inlineStr">
         <is>
-          <t>841 kcal</t>
+          <t>584 kcal</t>
         </is>
       </c>
       <c r="G17" s="0">
@@ -797,7 +797,7 @@
       </c>
       <c r="I17" s="0" t="inlineStr">
         <is>
-          <t>14/05/2021</t>
+          <t>12/07/2021</t>
         </is>
       </c>
     </row>
@@ -817,30 +817,30 @@
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
-          <t>R$ 176,86</t>
+          <t>R$ 178,17</t>
         </is>
       </c>
       <c r="E18" s="0" t="inlineStr">
         <is>
-          <t>R$ 203,39</t>
+          <t>R$ 204,90</t>
         </is>
       </c>
       <c r="F18" s="0" t="inlineStr">
         <is>
-          <t>857 kcal</t>
+          <t>357 kcal</t>
         </is>
       </c>
       <c r="G18" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="0" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I18" s="0" t="inlineStr">
         <is>
-          <t>30/04/2021</t>
+          <t>29/06/2021</t>
         </is>
       </c>
     </row>
@@ -860,21 +860,21 @@
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
-          <t>R$ 131,27</t>
+          <t>R$ 57,60</t>
         </is>
       </c>
       <c r="E19" s="0" t="inlineStr">
         <is>
-          <t>R$ 150,96</t>
+          <t>R$ 66,24</t>
         </is>
       </c>
       <c r="F19" s="0" t="inlineStr">
         <is>
-          <t>814 kcal</t>
+          <t>353 kcal</t>
         </is>
       </c>
       <c r="G19" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="0" t="inlineStr">
         <is>
@@ -883,7 +883,7 @@
       </c>
       <c r="I19" s="0" t="inlineStr">
         <is>
-          <t>20/05/2021</t>
+          <t>04/07/2021</t>
         </is>
       </c>
     </row>
@@ -903,30 +903,30 @@
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
-          <t>R$ 95,64</t>
+          <t>R$ 157,99</t>
         </is>
       </c>
       <c r="E20" s="0" t="inlineStr">
         <is>
-          <t>R$ 109,99</t>
+          <t>R$ 181,69</t>
         </is>
       </c>
       <c r="F20" s="0" t="inlineStr">
         <is>
-          <t>715 kcal</t>
+          <t>168 kcal</t>
         </is>
       </c>
       <c r="G20" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="0" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I20" s="0" t="inlineStr">
         <is>
-          <t>25/04/2021</t>
+          <t>19/06/2021</t>
         </is>
       </c>
     </row>
@@ -946,17 +946,17 @@
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
-          <t>R$ 145,34</t>
+          <t>R$ 142,57</t>
         </is>
       </c>
       <c r="E21" s="0" t="inlineStr">
         <is>
-          <t>R$ 167,14</t>
+          <t>R$ 163,96</t>
         </is>
       </c>
       <c r="F21" s="0" t="inlineStr">
         <is>
-          <t>643 kcal</t>
+          <t>635 kcal</t>
         </is>
       </c>
       <c r="G21" s="0">
@@ -964,12 +964,12 @@
       </c>
       <c r="H21" s="0" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I21" s="0" t="inlineStr">
         <is>
-          <t>05/05/2021</t>
+          <t>13/07/2021</t>
         </is>
       </c>
     </row>
@@ -989,30 +989,30 @@
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t>R$ 125,53</t>
+          <t>R$ 56,11</t>
         </is>
       </c>
       <c r="E22" s="0" t="inlineStr">
         <is>
-          <t>R$ 144,36</t>
+          <t>R$ 64,53</t>
         </is>
       </c>
       <c r="F22" s="0" t="inlineStr">
         <is>
-          <t>228 kcal</t>
+          <t>662 kcal</t>
         </is>
       </c>
       <c r="G22" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I22" s="0" t="inlineStr">
         <is>
-          <t>02/05/2021</t>
+          <t>01/07/2021</t>
         </is>
       </c>
     </row>
@@ -1032,17 +1032,17 @@
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t>R$ 118,03</t>
+          <t>R$ 198,60</t>
         </is>
       </c>
       <c r="E23" s="0" t="inlineStr">
         <is>
-          <t>R$ 135,73</t>
+          <t>R$ 228,39</t>
         </is>
       </c>
       <c r="F23" s="0" t="inlineStr">
         <is>
-          <t>686 kcal</t>
+          <t>558 kcal</t>
         </is>
       </c>
       <c r="G23" s="0">
@@ -1055,7 +1055,7 @@
       </c>
       <c r="I23" s="0" t="inlineStr">
         <is>
-          <t>22/04/2021</t>
+          <t>18/06/2021</t>
         </is>
       </c>
     </row>
@@ -1075,17 +1075,17 @@
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t>R$ 192,40</t>
+          <t>R$ 136,84</t>
         </is>
       </c>
       <c r="E24" s="0" t="inlineStr">
         <is>
-          <t>R$ 221,26</t>
+          <t>R$ 157,37</t>
         </is>
       </c>
       <c r="F24" s="0" t="inlineStr">
         <is>
-          <t>351 kcal</t>
+          <t>702 kcal</t>
         </is>
       </c>
       <c r="G24" s="0">
@@ -1093,12 +1093,12 @@
       </c>
       <c r="H24" s="0" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I24" s="0" t="inlineStr">
         <is>
-          <t>19/05/2021</t>
+          <t>15/07/2021</t>
         </is>
       </c>
     </row>
@@ -1118,17 +1118,17 @@
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
-          <t>R$ 102,68</t>
+          <t>R$ 97,51</t>
         </is>
       </c>
       <c r="E25" s="0" t="inlineStr">
         <is>
-          <t>R$ 118,08</t>
+          <t>R$ 112,14</t>
         </is>
       </c>
       <c r="F25" s="0" t="inlineStr">
         <is>
-          <t>864 kcal</t>
+          <t>551 kcal</t>
         </is>
       </c>
       <c r="G25" s="0">
@@ -1136,12 +1136,12 @@
       </c>
       <c r="H25" s="0" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I25" s="0" t="inlineStr">
         <is>
-          <t>27/04/2021</t>
+          <t>28/06/2021</t>
         </is>
       </c>
     </row>
@@ -1161,17 +1161,17 @@
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t>R$ 151,09</t>
+          <t>R$ 77,38</t>
         </is>
       </c>
       <c r="E26" s="0" t="inlineStr">
         <is>
-          <t>R$ 173,75</t>
+          <t>R$ 88,99</t>
         </is>
       </c>
       <c r="F26" s="0" t="inlineStr">
         <is>
-          <t>886 kcal</t>
+          <t>700 kcal</t>
         </is>
       </c>
       <c r="G26" s="0">
@@ -1179,12 +1179,12 @@
       </c>
       <c r="H26" s="0" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I26" s="0" t="inlineStr">
         <is>
-          <t>09/05/2021</t>
+          <t>18/06/2021</t>
         </is>
       </c>
     </row>
@@ -1204,17 +1204,17 @@
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t>R$ 92,46</t>
+          <t>R$ 58,93</t>
         </is>
       </c>
       <c r="E27" s="0" t="inlineStr">
         <is>
-          <t>R$ 106,33</t>
+          <t>R$ 67,77</t>
         </is>
       </c>
       <c r="F27" s="0" t="inlineStr">
         <is>
-          <t>567 kcal</t>
+          <t>485 kcal</t>
         </is>
       </c>
       <c r="G27" s="0">
@@ -1227,7 +1227,7 @@
       </c>
       <c r="I27" s="0" t="inlineStr">
         <is>
-          <t>24/04/2021</t>
+          <t>13/07/2021</t>
         </is>
       </c>
     </row>
@@ -1247,17 +1247,17 @@
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
-          <t>R$ 99,85</t>
+          <t>R$ 97,93</t>
         </is>
       </c>
       <c r="E28" s="0" t="inlineStr">
         <is>
-          <t>R$ 114,83</t>
+          <t>R$ 112,62</t>
         </is>
       </c>
       <c r="F28" s="0" t="inlineStr">
         <is>
-          <t>590 kcal</t>
+          <t>663 kcal</t>
         </is>
       </c>
       <c r="G28" s="0">
@@ -1265,12 +1265,12 @@
       </c>
       <c r="H28" s="0" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I28" s="0" t="inlineStr">
         <is>
-          <t>04/05/2021</t>
+          <t>30/06/2021</t>
         </is>
       </c>
     </row>
@@ -1290,30 +1290,30 @@
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
-          <t>R$ 139,96</t>
+          <t>R$ 85,81</t>
         </is>
       </c>
       <c r="E29" s="0" t="inlineStr">
         <is>
-          <t>R$ 160,95</t>
+          <t>R$ 98,68</t>
         </is>
       </c>
       <c r="F29" s="0" t="inlineStr">
         <is>
-          <t>377 kcal</t>
+          <t>83 kcal</t>
         </is>
       </c>
       <c r="G29" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="0" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I29" s="0" t="inlineStr">
         <is>
-          <t>30/04/2021</t>
+          <t>07/07/2021</t>
         </is>
       </c>
     </row>
@@ -1333,30 +1333,30 @@
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
-          <t>R$ 153,02</t>
+          <t>R$ 94,17</t>
         </is>
       </c>
       <c r="E30" s="0" t="inlineStr">
         <is>
-          <t>R$ 175,97</t>
+          <t>R$ 108,30</t>
         </is>
       </c>
       <c r="F30" s="0" t="inlineStr">
         <is>
-          <t>398 kcal</t>
+          <t>348 kcal</t>
         </is>
       </c>
       <c r="G30" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="0" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="I30" s="0" t="inlineStr">
         <is>
-          <t>08/05/2021</t>
+          <t>28/06/2021</t>
         </is>
       </c>
     </row>
@@ -1376,30 +1376,30 @@
       </c>
       <c r="D31" s="0" t="inlineStr">
         <is>
-          <t>R$ 151,35</t>
+          <t>R$ 66,44</t>
         </is>
       </c>
       <c r="E31" s="0" t="inlineStr">
         <is>
-          <t>R$ 174,05</t>
+          <t>R$ 76,41</t>
         </is>
       </c>
       <c r="F31" s="0" t="inlineStr">
         <is>
-          <t>705 kcal</t>
+          <t>860 kcal</t>
         </is>
       </c>
       <c r="G31" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I31" s="0" t="inlineStr">
         <is>
-          <t>11/05/2021</t>
+          <t>21/06/2021</t>
         </is>
       </c>
     </row>
@@ -1419,17 +1419,17 @@
       </c>
       <c r="D32" s="0" t="inlineStr">
         <is>
-          <t>R$ 130,90</t>
+          <t>R$ 76,21</t>
         </is>
       </c>
       <c r="E32" s="0" t="inlineStr">
         <is>
-          <t>R$ 150,54</t>
+          <t>R$ 87,64</t>
         </is>
       </c>
       <c r="F32" s="0" t="inlineStr">
         <is>
-          <t>324 kcal</t>
+          <t>193 kcal</t>
         </is>
       </c>
       <c r="G32" s="0">
@@ -1437,12 +1437,12 @@
       </c>
       <c r="H32" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="I32" s="0" t="inlineStr">
         <is>
-          <t>11/05/2021</t>
+          <t>01/07/2021</t>
         </is>
       </c>
     </row>
@@ -1462,30 +1462,30 @@
       </c>
       <c r="D33" s="0" t="inlineStr">
         <is>
-          <t>R$ 67,65</t>
+          <t>R$ 92,52</t>
         </is>
       </c>
       <c r="E33" s="0" t="inlineStr">
         <is>
-          <t>R$ 77,80</t>
+          <t>R$ 106,40</t>
         </is>
       </c>
       <c r="F33" s="0" t="inlineStr">
         <is>
-          <t>705 kcal</t>
+          <t>293 kcal</t>
         </is>
       </c>
       <c r="G33" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" s="0" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="I33" s="0" t="inlineStr">
         <is>
-          <t>20/05/2021</t>
+          <t>07/07/2021</t>
         </is>
       </c>
     </row>
@@ -1505,17 +1505,17 @@
       </c>
       <c r="D34" s="0" t="inlineStr">
         <is>
-          <t>R$ 191,46</t>
+          <t>R$ 178,43</t>
         </is>
       </c>
       <c r="E34" s="0" t="inlineStr">
         <is>
-          <t>R$ 220,18</t>
+          <t>R$ 205,19</t>
         </is>
       </c>
       <c r="F34" s="0" t="inlineStr">
         <is>
-          <t>179 kcal</t>
+          <t>309 kcal</t>
         </is>
       </c>
       <c r="G34" s="0">
@@ -1523,12 +1523,12 @@
       </c>
       <c r="H34" s="0" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I34" s="0" t="inlineStr">
         <is>
-          <t>25/04/2021</t>
+          <t>23/06/2021</t>
         </is>
       </c>
     </row>
@@ -1548,30 +1548,30 @@
       </c>
       <c r="D35" s="0" t="inlineStr">
         <is>
-          <t>R$ 178,57</t>
+          <t>R$ 108,58</t>
         </is>
       </c>
       <c r="E35" s="0" t="inlineStr">
         <is>
-          <t>R$ 205,36</t>
+          <t>R$ 124,87</t>
         </is>
       </c>
       <c r="F35" s="0" t="inlineStr">
         <is>
-          <t>332 kcal</t>
+          <t>776 kcal</t>
         </is>
       </c>
       <c r="G35" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I35" s="0" t="inlineStr">
         <is>
-          <t>08/05/2021</t>
+          <t>02/07/2021</t>
         </is>
       </c>
     </row>
@@ -1591,30 +1591,30 @@
       </c>
       <c r="D36" s="0" t="inlineStr">
         <is>
-          <t>R$ 116,75</t>
+          <t>R$ 165,17</t>
         </is>
       </c>
       <c r="E36" s="0" t="inlineStr">
         <is>
-          <t>R$ 134,26</t>
+          <t>R$ 189,95</t>
         </is>
       </c>
       <c r="F36" s="0" t="inlineStr">
         <is>
-          <t>312 kcal</t>
+          <t>626 kcal</t>
         </is>
       </c>
       <c r="G36" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36" s="0" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I36" s="0" t="inlineStr">
         <is>
-          <t>15/05/2021</t>
+          <t>15/07/2021</t>
         </is>
       </c>
     </row>
@@ -1634,21 +1634,21 @@
       </c>
       <c r="D37" s="0" t="inlineStr">
         <is>
-          <t>R$ 190,96</t>
+          <t>R$ 69,27</t>
         </is>
       </c>
       <c r="E37" s="0" t="inlineStr">
         <is>
-          <t>R$ 219,60</t>
+          <t>R$ 79,66</t>
         </is>
       </c>
       <c r="F37" s="0" t="inlineStr">
         <is>
-          <t>488 kcal</t>
+          <t>877 kcal</t>
         </is>
       </c>
       <c r="G37" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37" s="0" t="inlineStr">
         <is>
@@ -1657,7 +1657,7 @@
       </c>
       <c r="I37" s="0" t="inlineStr">
         <is>
-          <t>03/05/2021</t>
+          <t>07/07/2021</t>
         </is>
       </c>
     </row>
@@ -1677,17 +1677,17 @@
       </c>
       <c r="D38" s="0" t="inlineStr">
         <is>
-          <t>R$ 172,62</t>
+          <t>R$ 174,96</t>
         </is>
       </c>
       <c r="E38" s="0" t="inlineStr">
         <is>
-          <t>R$ 198,51</t>
+          <t>R$ 201,20</t>
         </is>
       </c>
       <c r="F38" s="0" t="inlineStr">
         <is>
-          <t>718 kcal</t>
+          <t>575 kcal</t>
         </is>
       </c>
       <c r="G38" s="0">
@@ -1695,12 +1695,12 @@
       </c>
       <c r="H38" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I38" s="0" t="inlineStr">
         <is>
-          <t>29/04/2021</t>
+          <t>26/06/2021</t>
         </is>
       </c>
     </row>
@@ -1720,17 +1720,17 @@
       </c>
       <c r="D39" s="0" t="inlineStr">
         <is>
-          <t>R$ 58,43</t>
+          <t>R$ 172,79</t>
         </is>
       </c>
       <c r="E39" s="0" t="inlineStr">
         <is>
-          <t>R$ 67,19</t>
+          <t>R$ 198,71</t>
         </is>
       </c>
       <c r="F39" s="0" t="inlineStr">
         <is>
-          <t>256 kcal</t>
+          <t>89 kcal</t>
         </is>
       </c>
       <c r="G39" s="0">
@@ -1743,7 +1743,7 @@
       </c>
       <c r="I39" s="0" t="inlineStr">
         <is>
-          <t>24/04/2021</t>
+          <t>15/07/2021</t>
         </is>
       </c>
     </row>
@@ -1763,17 +1763,17 @@
       </c>
       <c r="D40" s="0" t="inlineStr">
         <is>
-          <t>R$ 76,82</t>
+          <t>R$ 108,23</t>
         </is>
       </c>
       <c r="E40" s="0" t="inlineStr">
         <is>
-          <t>R$ 88,34</t>
+          <t>R$ 124,46</t>
         </is>
       </c>
       <c r="F40" s="0" t="inlineStr">
         <is>
-          <t>589 kcal</t>
+          <t>719 kcal</t>
         </is>
       </c>
       <c r="G40" s="0">
@@ -1781,12 +1781,12 @@
       </c>
       <c r="H40" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I40" s="0" t="inlineStr">
         <is>
-          <t>21/05/2021</t>
+          <t>06/07/2021</t>
         </is>
       </c>
     </row>
@@ -1806,21 +1806,21 @@
       </c>
       <c r="D41" s="0" t="inlineStr">
         <is>
-          <t>R$ 179,39</t>
+          <t>R$ 94,93</t>
         </is>
       </c>
       <c r="E41" s="0" t="inlineStr">
         <is>
-          <t>R$ 206,30</t>
+          <t>R$ 109,17</t>
         </is>
       </c>
       <c r="F41" s="0" t="inlineStr">
         <is>
-          <t>315 kcal</t>
+          <t>595 kcal</t>
         </is>
       </c>
       <c r="G41" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="0" t="inlineStr">
         <is>
@@ -1829,7 +1829,7 @@
       </c>
       <c r="I41" s="0" t="inlineStr">
         <is>
-          <t>30/04/2021</t>
+          <t>29/06/2021</t>
         </is>
       </c>
     </row>
@@ -1849,17 +1849,17 @@
       </c>
       <c r="D42" s="0" t="inlineStr">
         <is>
-          <t>R$ 86,29</t>
+          <t>R$ 107,50</t>
         </is>
       </c>
       <c r="E42" s="0" t="inlineStr">
         <is>
-          <t>R$ 99,23</t>
+          <t>R$ 123,63</t>
         </is>
       </c>
       <c r="F42" s="0" t="inlineStr">
         <is>
-          <t>333 kcal</t>
+          <t>816 kcal</t>
         </is>
       </c>
       <c r="G42" s="0">
@@ -1867,12 +1867,12 @@
       </c>
       <c r="H42" s="0" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="I42" s="0" t="inlineStr">
         <is>
-          <t>07/05/2021</t>
+          <t>19/06/2021</t>
         </is>
       </c>
     </row>
@@ -1892,30 +1892,30 @@
       </c>
       <c r="D43" s="0" t="inlineStr">
         <is>
-          <t>R$ 70,97</t>
+          <t>R$ 199,93</t>
         </is>
       </c>
       <c r="E43" s="0" t="inlineStr">
         <is>
-          <t>R$ 81,62</t>
+          <t>R$ 229,92</t>
         </is>
       </c>
       <c r="F43" s="0" t="inlineStr">
         <is>
-          <t>347 kcal</t>
+          <t>367 kcal</t>
         </is>
       </c>
       <c r="G43" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="I43" s="0" t="inlineStr">
         <is>
-          <t>04/05/2021</t>
+          <t>23/06/2021</t>
         </is>
       </c>
     </row>
@@ -1935,30 +1935,30 @@
       </c>
       <c r="D44" s="0" t="inlineStr">
         <is>
-          <t>R$ 81,18</t>
+          <t>R$ 115,00</t>
         </is>
       </c>
       <c r="E44" s="0" t="inlineStr">
         <is>
-          <t>R$ 93,36</t>
+          <t>R$ 132,25</t>
         </is>
       </c>
       <c r="F44" s="0" t="inlineStr">
         <is>
-          <t>640 kcal</t>
+          <t>294 kcal</t>
         </is>
       </c>
       <c r="G44" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I44" s="0" t="inlineStr">
         <is>
-          <t>28/04/2021</t>
+          <t>30/06/2021</t>
         </is>
       </c>
     </row>
@@ -1978,17 +1978,17 @@
       </c>
       <c r="D45" s="0" t="inlineStr">
         <is>
-          <t>R$ 162,91</t>
+          <t>R$ 59,88</t>
         </is>
       </c>
       <c r="E45" s="0" t="inlineStr">
         <is>
-          <t>R$ 187,35</t>
+          <t>R$ 68,86</t>
         </is>
       </c>
       <c r="F45" s="0" t="inlineStr">
         <is>
-          <t>774 kcal</t>
+          <t>614 kcal</t>
         </is>
       </c>
       <c r="G45" s="0">
@@ -1996,12 +1996,12 @@
       </c>
       <c r="H45" s="0" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I45" s="0" t="inlineStr">
         <is>
-          <t>07/05/2021</t>
+          <t>28/06/2021</t>
         </is>
       </c>
     </row>
@@ -2021,17 +2021,17 @@
       </c>
       <c r="D46" s="0" t="inlineStr">
         <is>
-          <t>R$ 70,21</t>
+          <t>R$ 91,00</t>
         </is>
       </c>
       <c r="E46" s="0" t="inlineStr">
         <is>
-          <t>R$ 80,74</t>
+          <t>R$ 104,65</t>
         </is>
       </c>
       <c r="F46" s="0" t="inlineStr">
         <is>
-          <t>297 kcal</t>
+          <t>651 kcal</t>
         </is>
       </c>
       <c r="G46" s="0">
@@ -2039,12 +2039,12 @@
       </c>
       <c r="H46" s="0" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I46" s="0" t="inlineStr">
         <is>
-          <t>12/05/2021</t>
+          <t>13/07/2021</t>
         </is>
       </c>
     </row>
@@ -2064,30 +2064,30 @@
       </c>
       <c r="D47" s="0" t="inlineStr">
         <is>
-          <t>R$ 120,23</t>
+          <t>R$ 149,30</t>
         </is>
       </c>
       <c r="E47" s="0" t="inlineStr">
         <is>
-          <t>R$ 138,26</t>
+          <t>R$ 171,70</t>
         </is>
       </c>
       <c r="F47" s="0" t="inlineStr">
         <is>
-          <t>384 kcal</t>
+          <t>881 kcal</t>
         </is>
       </c>
       <c r="G47" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47" s="0" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="I47" s="0" t="inlineStr">
         <is>
-          <t>09/05/2021</t>
+          <t>18/06/2021</t>
         </is>
       </c>
     </row>
@@ -2107,17 +2107,17 @@
       </c>
       <c r="D48" s="0" t="inlineStr">
         <is>
-          <t>R$ 120,94</t>
+          <t>R$ 170,08</t>
         </is>
       </c>
       <c r="E48" s="0" t="inlineStr">
         <is>
-          <t>R$ 139,08</t>
+          <t>R$ 195,59</t>
         </is>
       </c>
       <c r="F48" s="0" t="inlineStr">
         <is>
-          <t>584 kcal</t>
+          <t>436 kcal</t>
         </is>
       </c>
       <c r="G48" s="0">
@@ -2125,12 +2125,12 @@
       </c>
       <c r="H48" s="0" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="I48" s="0" t="inlineStr">
         <is>
-          <t>05/05/2021</t>
+          <t>12/07/2021</t>
         </is>
       </c>
     </row>
@@ -2150,17 +2150,17 @@
       </c>
       <c r="D49" s="0" t="inlineStr">
         <is>
-          <t>R$ 84,21</t>
+          <t>R$ 179,47</t>
         </is>
       </c>
       <c r="E49" s="0" t="inlineStr">
         <is>
-          <t>R$ 96,84</t>
+          <t>R$ 206,39</t>
         </is>
       </c>
       <c r="F49" s="0" t="inlineStr">
         <is>
-          <t>440 kcal</t>
+          <t>521 kcal</t>
         </is>
       </c>
       <c r="G49" s="0">
@@ -2168,12 +2168,12 @@
       </c>
       <c r="H49" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I49" s="0" t="inlineStr">
         <is>
-          <t>19/05/2021</t>
+          <t>25/06/2021</t>
         </is>
       </c>
     </row>
@@ -2193,17 +2193,17 @@
       </c>
       <c r="D50" s="0" t="inlineStr">
         <is>
-          <t>R$ 82,29</t>
+          <t>R$ 79,40</t>
         </is>
       </c>
       <c r="E50" s="0" t="inlineStr">
         <is>
-          <t>R$ 94,63</t>
+          <t>R$ 91,31</t>
         </is>
       </c>
       <c r="F50" s="0" t="inlineStr">
         <is>
-          <t>685 kcal</t>
+          <t>745 kcal</t>
         </is>
       </c>
       <c r="G50" s="0">
@@ -2211,12 +2211,12 @@
       </c>
       <c r="H50" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I50" s="0" t="inlineStr">
         <is>
-          <t>11/05/2021</t>
+          <t>17/06/2021</t>
         </is>
       </c>
     </row>
@@ -2236,17 +2236,17 @@
       </c>
       <c r="D51" s="0" t="inlineStr">
         <is>
-          <t>R$ 77,21</t>
+          <t>R$ 94,51</t>
         </is>
       </c>
       <c r="E51" s="0" t="inlineStr">
         <is>
-          <t>R$ 88,79</t>
+          <t>R$ 108,69</t>
         </is>
       </c>
       <c r="F51" s="0" t="inlineStr">
         <is>
-          <t>315 kcal</t>
+          <t>680 kcal</t>
         </is>
       </c>
       <c r="G51" s="0">
@@ -2254,12 +2254,12 @@
       </c>
       <c r="H51" s="0" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I51" s="0" t="inlineStr">
         <is>
-          <t>13/05/2021</t>
+          <t>22/06/2021</t>
         </is>
       </c>
     </row>
@@ -2279,17 +2279,17 @@
       </c>
       <c r="D52" s="0" t="inlineStr">
         <is>
-          <t>R$ 112,63</t>
+          <t>R$ 121,05</t>
         </is>
       </c>
       <c r="E52" s="0" t="inlineStr">
         <is>
-          <t>R$ 129,52</t>
+          <t>R$ 139,21</t>
         </is>
       </c>
       <c r="F52" s="0" t="inlineStr">
         <is>
-          <t>885 kcal</t>
+          <t>532 kcal</t>
         </is>
       </c>
       <c r="G52" s="0">
@@ -2297,12 +2297,12 @@
       </c>
       <c r="H52" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I52" s="0" t="inlineStr">
         <is>
-          <t>16/05/2021</t>
+          <t>27/06/2021</t>
         </is>
       </c>
     </row>
@@ -2322,17 +2322,17 @@
       </c>
       <c r="D53" s="0" t="inlineStr">
         <is>
-          <t>R$ 67,25</t>
+          <t>R$ 141,45</t>
         </is>
       </c>
       <c r="E53" s="0" t="inlineStr">
         <is>
-          <t>R$ 77,34</t>
+          <t>R$ 162,67</t>
         </is>
       </c>
       <c r="F53" s="0" t="inlineStr">
         <is>
-          <t>322 kcal</t>
+          <t>280 kcal</t>
         </is>
       </c>
       <c r="G53" s="0">
@@ -2340,12 +2340,12 @@
       </c>
       <c r="H53" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I53" s="0" t="inlineStr">
         <is>
-          <t>28/04/2021</t>
+          <t>23/06/2021</t>
         </is>
       </c>
     </row>
@@ -2365,30 +2365,30 @@
       </c>
       <c r="D54" s="0" t="inlineStr">
         <is>
-          <t>R$ 156,01</t>
+          <t>R$ 157,02</t>
         </is>
       </c>
       <c r="E54" s="0" t="inlineStr">
         <is>
-          <t>R$ 179,41</t>
+          <t>R$ 180,57</t>
         </is>
       </c>
       <c r="F54" s="0" t="inlineStr">
         <is>
-          <t>84 kcal</t>
+          <t>158 kcal</t>
         </is>
       </c>
       <c r="G54" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H54" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I54" s="0" t="inlineStr">
         <is>
-          <t>12/05/2021</t>
+          <t>02/07/2021</t>
         </is>
       </c>
     </row>
@@ -2408,17 +2408,17 @@
       </c>
       <c r="D55" s="0" t="inlineStr">
         <is>
-          <t>R$ 191,96</t>
+          <t>R$ 151,15</t>
         </is>
       </c>
       <c r="E55" s="0" t="inlineStr">
         <is>
-          <t>R$ 220,75</t>
+          <t>R$ 173,82</t>
         </is>
       </c>
       <c r="F55" s="0" t="inlineStr">
         <is>
-          <t>769 kcal</t>
+          <t>552 kcal</t>
         </is>
       </c>
       <c r="G55" s="0">
@@ -2431,7 +2431,7 @@
       </c>
       <c r="I55" s="0" t="inlineStr">
         <is>
-          <t>22/04/2021</t>
+          <t>17/06/2021</t>
         </is>
       </c>
     </row>
@@ -2451,17 +2451,17 @@
       </c>
       <c r="D56" s="0" t="inlineStr">
         <is>
-          <t>R$ 53,76</t>
+          <t>R$ 90,65</t>
         </is>
       </c>
       <c r="E56" s="0" t="inlineStr">
         <is>
-          <t>R$ 61,82</t>
+          <t>R$ 104,25</t>
         </is>
       </c>
       <c r="F56" s="0" t="inlineStr">
         <is>
-          <t>450 kcal</t>
+          <t>883 kcal</t>
         </is>
       </c>
       <c r="G56" s="0">
@@ -2469,12 +2469,12 @@
       </c>
       <c r="H56" s="0" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="I56" s="0" t="inlineStr">
         <is>
-          <t>03/05/2021</t>
+          <t>28/06/2021</t>
         </is>
       </c>
     </row>
@@ -2494,17 +2494,17 @@
       </c>
       <c r="D57" s="0" t="inlineStr">
         <is>
-          <t>R$ 192,46</t>
+          <t>R$ 107,57</t>
         </is>
       </c>
       <c r="E57" s="0" t="inlineStr">
         <is>
-          <t>R$ 221,33</t>
+          <t>R$ 123,71</t>
         </is>
       </c>
       <c r="F57" s="0" t="inlineStr">
         <is>
-          <t>779 kcal</t>
+          <t>280 kcal</t>
         </is>
       </c>
       <c r="G57" s="0">
@@ -2512,12 +2512,12 @@
       </c>
       <c r="H57" s="0" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I57" s="0" t="inlineStr">
         <is>
-          <t>12/05/2021</t>
+          <t>03/07/2021</t>
         </is>
       </c>
     </row>
@@ -2537,17 +2537,17 @@
       </c>
       <c r="D58" s="0" t="inlineStr">
         <is>
-          <t>R$ 108,52</t>
+          <t>R$ 192,60</t>
         </is>
       </c>
       <c r="E58" s="0" t="inlineStr">
         <is>
-          <t>R$ 124,80</t>
+          <t>R$ 221,49</t>
         </is>
       </c>
       <c r="F58" s="0" t="inlineStr">
         <is>
-          <t>757 kcal</t>
+          <t>802 kcal</t>
         </is>
       </c>
       <c r="G58" s="0">
@@ -2555,12 +2555,12 @@
       </c>
       <c r="H58" s="0" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="I58" s="0" t="inlineStr">
         <is>
-          <t>24/04/2021</t>
+          <t>30/06/2021</t>
         </is>
       </c>
     </row>
@@ -2580,21 +2580,21 @@
       </c>
       <c r="D59" s="0" t="inlineStr">
         <is>
-          <t>R$ 190,50</t>
+          <t>R$ 126,78</t>
         </is>
       </c>
       <c r="E59" s="0" t="inlineStr">
         <is>
-          <t>R$ 219,08</t>
+          <t>R$ 145,80</t>
         </is>
       </c>
       <c r="F59" s="0" t="inlineStr">
         <is>
-          <t>865 kcal</t>
+          <t>389 kcal</t>
         </is>
       </c>
       <c r="G59" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H59" s="0" t="inlineStr">
         <is>
@@ -2603,7 +2603,7 @@
       </c>
       <c r="I59" s="0" t="inlineStr">
         <is>
-          <t>05/05/2021</t>
+          <t>28/06/2021</t>
         </is>
       </c>
     </row>
@@ -2623,17 +2623,17 @@
       </c>
       <c r="D60" s="0" t="inlineStr">
         <is>
-          <t>R$ 169,07</t>
+          <t>R$ 87,19</t>
         </is>
       </c>
       <c r="E60" s="0" t="inlineStr">
         <is>
-          <t>R$ 194,43</t>
+          <t>R$ 100,27</t>
         </is>
       </c>
       <c r="F60" s="0" t="inlineStr">
         <is>
-          <t>837 kcal</t>
+          <t>562 kcal</t>
         </is>
       </c>
       <c r="G60" s="0">
@@ -2646,7 +2646,7 @@
       </c>
       <c r="I60" s="0" t="inlineStr">
         <is>
-          <t>04/05/2021</t>
+          <t>27/06/2021</t>
         </is>
       </c>
     </row>
@@ -2666,30 +2666,30 @@
       </c>
       <c r="D61" s="0" t="inlineStr">
         <is>
-          <t>R$ 92,78</t>
+          <t>R$ 124,46</t>
         </is>
       </c>
       <c r="E61" s="0" t="inlineStr">
         <is>
-          <t>R$ 106,70</t>
+          <t>R$ 143,13</t>
         </is>
       </c>
       <c r="F61" s="0" t="inlineStr">
         <is>
-          <t>510 kcal</t>
+          <t>667 kcal</t>
         </is>
       </c>
       <c r="G61" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H61" s="0" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I61" s="0" t="inlineStr">
         <is>
-          <t>19/05/2021</t>
+          <t>23/06/2021</t>
         </is>
       </c>
     </row>
@@ -2709,30 +2709,30 @@
       </c>
       <c r="D62" s="0" t="inlineStr">
         <is>
-          <t>R$ 116,41</t>
+          <t>R$ 115,06</t>
         </is>
       </c>
       <c r="E62" s="0" t="inlineStr">
         <is>
-          <t>R$ 133,87</t>
+          <t>R$ 132,32</t>
         </is>
       </c>
       <c r="F62" s="0" t="inlineStr">
         <is>
-          <t>492 kcal</t>
+          <t>406 kcal</t>
         </is>
       </c>
       <c r="G62" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62" s="0" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="I62" s="0" t="inlineStr">
         <is>
-          <t>03/05/2021</t>
+          <t>03/07/2021</t>
         </is>
       </c>
     </row>
@@ -2752,17 +2752,17 @@
       </c>
       <c r="D63" s="0" t="inlineStr">
         <is>
-          <t>R$ 149,25</t>
+          <t>R$ 176,80</t>
         </is>
       </c>
       <c r="E63" s="0" t="inlineStr">
         <is>
-          <t>R$ 171,64</t>
+          <t>R$ 203,32</t>
         </is>
       </c>
       <c r="F63" s="0" t="inlineStr">
         <is>
-          <t>146 kcal</t>
+          <t>299 kcal</t>
         </is>
       </c>
       <c r="G63" s="0">
@@ -2770,12 +2770,12 @@
       </c>
       <c r="H63" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="I63" s="0" t="inlineStr">
         <is>
-          <t>04/05/2021</t>
+          <t>21/06/2021</t>
         </is>
       </c>
     </row>
@@ -2795,17 +2795,17 @@
       </c>
       <c r="D64" s="0" t="inlineStr">
         <is>
-          <t>R$ 182,44</t>
+          <t>R$ 190,75</t>
         </is>
       </c>
       <c r="E64" s="0" t="inlineStr">
         <is>
-          <t>R$ 209,81</t>
+          <t>R$ 219,36</t>
         </is>
       </c>
       <c r="F64" s="0" t="inlineStr">
         <is>
-          <t>632 kcal</t>
+          <t>808 kcal</t>
         </is>
       </c>
       <c r="G64" s="0">
@@ -2813,12 +2813,12 @@
       </c>
       <c r="H64" s="0" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I64" s="0" t="inlineStr">
         <is>
-          <t>13/05/2021</t>
+          <t>04/07/2021</t>
         </is>
       </c>
     </row>
@@ -2838,21 +2838,21 @@
       </c>
       <c r="D65" s="0" t="inlineStr">
         <is>
-          <t>R$ 52,32</t>
+          <t>R$ 178,08</t>
         </is>
       </c>
       <c r="E65" s="0" t="inlineStr">
         <is>
-          <t>R$ 60,17</t>
+          <t>R$ 204,79</t>
         </is>
       </c>
       <c r="F65" s="0" t="inlineStr">
         <is>
-          <t>250 kcal</t>
+          <t>486 kcal</t>
         </is>
       </c>
       <c r="G65" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H65" s="0" t="inlineStr">
         <is>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="I65" s="0" t="inlineStr">
         <is>
-          <t>26/04/2021</t>
+          <t>14/07/2021</t>
         </is>
       </c>
     </row>
@@ -2881,17 +2881,17 @@
       </c>
       <c r="D66" s="0" t="inlineStr">
         <is>
-          <t>R$ 84,69</t>
+          <t>R$ 67,95</t>
         </is>
       </c>
       <c r="E66" s="0" t="inlineStr">
         <is>
-          <t>R$ 97,39</t>
+          <t>R$ 78,14</t>
         </is>
       </c>
       <c r="F66" s="0" t="inlineStr">
         <is>
-          <t>873 kcal</t>
+          <t>140 kcal</t>
         </is>
       </c>
       <c r="G66" s="0">
@@ -2904,7 +2904,7 @@
       </c>
       <c r="I66" s="0" t="inlineStr">
         <is>
-          <t>02/05/2021</t>
+          <t>17/06/2021</t>
         </is>
       </c>
     </row>
@@ -2924,21 +2924,21 @@
       </c>
       <c r="D67" s="0" t="inlineStr">
         <is>
-          <t>R$ 176,11</t>
+          <t>R$ 174,99</t>
         </is>
       </c>
       <c r="E67" s="0" t="inlineStr">
         <is>
-          <t>R$ 202,53</t>
+          <t>R$ 201,24</t>
         </is>
       </c>
       <c r="F67" s="0" t="inlineStr">
         <is>
-          <t>273 kcal</t>
+          <t>545 kcal</t>
         </is>
       </c>
       <c r="G67" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67" s="0" t="inlineStr">
         <is>
@@ -2947,7 +2947,7 @@
       </c>
       <c r="I67" s="0" t="inlineStr">
         <is>
-          <t>20/05/2021</t>
+          <t>07/07/2021</t>
         </is>
       </c>
     </row>
@@ -2967,17 +2967,17 @@
       </c>
       <c r="D68" s="0" t="inlineStr">
         <is>
-          <t>R$ 65,90</t>
+          <t>R$ 169,06</t>
         </is>
       </c>
       <c r="E68" s="0" t="inlineStr">
         <is>
-          <t>R$ 75,79</t>
+          <t>R$ 194,42</t>
         </is>
       </c>
       <c r="F68" s="0" t="inlineStr">
         <is>
-          <t>526 kcal</t>
+          <t>390 kcal</t>
         </is>
       </c>
       <c r="G68" s="0">
@@ -2985,12 +2985,12 @@
       </c>
       <c r="H68" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I68" s="0" t="inlineStr">
         <is>
-          <t>06/05/2021</t>
+          <t>11/07/2021</t>
         </is>
       </c>
     </row>
@@ -3010,17 +3010,17 @@
       </c>
       <c r="D69" s="0" t="inlineStr">
         <is>
-          <t>R$ 115,56</t>
+          <t>R$ 122,24</t>
         </is>
       </c>
       <c r="E69" s="0" t="inlineStr">
         <is>
-          <t>R$ 132,89</t>
+          <t>R$ 140,58</t>
         </is>
       </c>
       <c r="F69" s="0" t="inlineStr">
         <is>
-          <t>768 kcal</t>
+          <t>857 kcal</t>
         </is>
       </c>
       <c r="G69" s="0">
@@ -3028,12 +3028,12 @@
       </c>
       <c r="H69" s="0" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I69" s="0" t="inlineStr">
         <is>
-          <t>28/04/2021</t>
+          <t>01/07/2021</t>
         </is>
       </c>
     </row>
@@ -3053,30 +3053,30 @@
       </c>
       <c r="D70" s="0" t="inlineStr">
         <is>
-          <t>R$ 83,91</t>
+          <t>R$ 89,63</t>
         </is>
       </c>
       <c r="E70" s="0" t="inlineStr">
         <is>
-          <t>R$ 96,50</t>
+          <t>R$ 103,07</t>
         </is>
       </c>
       <c r="F70" s="0" t="inlineStr">
         <is>
-          <t>796 kcal</t>
+          <t>538 kcal</t>
         </is>
       </c>
       <c r="G70" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H70" s="0" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I70" s="0" t="inlineStr">
         <is>
-          <t>07/05/2021</t>
+          <t>27/06/2021</t>
         </is>
       </c>
     </row>
@@ -3096,21 +3096,21 @@
       </c>
       <c r="D71" s="0" t="inlineStr">
         <is>
-          <t>R$ 91,36</t>
+          <t>R$ 160,58</t>
         </is>
       </c>
       <c r="E71" s="0" t="inlineStr">
         <is>
-          <t>R$ 105,06</t>
+          <t>R$ 184,67</t>
         </is>
       </c>
       <c r="F71" s="0" t="inlineStr">
         <is>
-          <t>732 kcal</t>
+          <t>571 kcal</t>
         </is>
       </c>
       <c r="G71" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H71" s="0" t="inlineStr">
         <is>
@@ -3119,7 +3119,7 @@
       </c>
       <c r="I71" s="0" t="inlineStr">
         <is>
-          <t>01/05/2021</t>
+          <t>14/07/2021</t>
         </is>
       </c>
     </row>
@@ -3139,21 +3139,21 @@
       </c>
       <c r="D72" s="0" t="inlineStr">
         <is>
-          <t>R$ 145,66</t>
+          <t>R$ 124,64</t>
         </is>
       </c>
       <c r="E72" s="0" t="inlineStr">
         <is>
-          <t>R$ 167,51</t>
+          <t>R$ 143,34</t>
         </is>
       </c>
       <c r="F72" s="0" t="inlineStr">
         <is>
-          <t>727 kcal</t>
+          <t>692 kcal</t>
         </is>
       </c>
       <c r="G72" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H72" s="0" t="inlineStr">
         <is>
@@ -3162,7 +3162,7 @@
       </c>
       <c r="I72" s="0" t="inlineStr">
         <is>
-          <t>29/04/2021</t>
+          <t>12/07/2021</t>
         </is>
       </c>
     </row>
@@ -3182,21 +3182,21 @@
       </c>
       <c r="D73" s="0" t="inlineStr">
         <is>
-          <t>R$ 180,28</t>
+          <t>R$ 168,52</t>
         </is>
       </c>
       <c r="E73" s="0" t="inlineStr">
         <is>
-          <t>R$ 207,32</t>
+          <t>R$ 193,80</t>
         </is>
       </c>
       <c r="F73" s="0" t="inlineStr">
         <is>
-          <t>748 kcal</t>
+          <t>377 kcal</t>
         </is>
       </c>
       <c r="G73" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73" s="0" t="inlineStr">
         <is>
@@ -3205,7 +3205,7 @@
       </c>
       <c r="I73" s="0" t="inlineStr">
         <is>
-          <t>07/05/2021</t>
+          <t>15/07/2021</t>
         </is>
       </c>
     </row>
@@ -3225,30 +3225,30 @@
       </c>
       <c r="D74" s="0" t="inlineStr">
         <is>
-          <t>R$ 114,86</t>
+          <t>R$ 169,70</t>
         </is>
       </c>
       <c r="E74" s="0" t="inlineStr">
         <is>
-          <t>R$ 132,09</t>
+          <t>R$ 195,16</t>
         </is>
       </c>
       <c r="F74" s="0" t="inlineStr">
         <is>
-          <t>734 kcal</t>
+          <t>822 kcal</t>
         </is>
       </c>
       <c r="G74" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H74" s="0" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I74" s="0" t="inlineStr">
         <is>
-          <t>13/05/2021</t>
+          <t>19/06/2021</t>
         </is>
       </c>
     </row>
@@ -3268,17 +3268,17 @@
       </c>
       <c r="D75" s="0" t="inlineStr">
         <is>
-          <t>R$ 128,06</t>
+          <t>R$ 171,63</t>
         </is>
       </c>
       <c r="E75" s="0" t="inlineStr">
         <is>
-          <t>R$ 147,27</t>
+          <t>R$ 197,37</t>
         </is>
       </c>
       <c r="F75" s="0" t="inlineStr">
         <is>
-          <t>852 kcal</t>
+          <t>396 kcal</t>
         </is>
       </c>
       <c r="G75" s="0">
@@ -3286,12 +3286,12 @@
       </c>
       <c r="H75" s="0" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I75" s="0" t="inlineStr">
         <is>
-          <t>07/05/2021</t>
+          <t>15/07/2021</t>
         </is>
       </c>
     </row>
@@ -3311,17 +3311,17 @@
       </c>
       <c r="D76" s="0" t="inlineStr">
         <is>
-          <t>R$ 77,10</t>
+          <t>R$ 138,14</t>
         </is>
       </c>
       <c r="E76" s="0" t="inlineStr">
         <is>
-          <t>R$ 88,67</t>
+          <t>R$ 158,86</t>
         </is>
       </c>
       <c r="F76" s="0" t="inlineStr">
         <is>
-          <t>196 kcal</t>
+          <t>301 kcal</t>
         </is>
       </c>
       <c r="G76" s="0">
@@ -3334,7 +3334,7 @@
       </c>
       <c r="I76" s="0" t="inlineStr">
         <is>
-          <t>29/04/2021</t>
+          <t>26/06/2021</t>
         </is>
       </c>
     </row>
@@ -3354,17 +3354,17 @@
       </c>
       <c r="D77" s="0" t="inlineStr">
         <is>
-          <t>R$ 89,41</t>
+          <t>R$ 93,11</t>
         </is>
       </c>
       <c r="E77" s="0" t="inlineStr">
         <is>
-          <t>R$ 102,82</t>
+          <t>R$ 107,08</t>
         </is>
       </c>
       <c r="F77" s="0" t="inlineStr">
         <is>
-          <t>412 kcal</t>
+          <t>645 kcal</t>
         </is>
       </c>
       <c r="G77" s="0">
@@ -3377,7 +3377,7 @@
       </c>
       <c r="I77" s="0" t="inlineStr">
         <is>
-          <t>23/04/2021</t>
+          <t>11/07/2021</t>
         </is>
       </c>
     </row>
@@ -3397,21 +3397,21 @@
       </c>
       <c r="D78" s="0" t="inlineStr">
         <is>
-          <t>R$ 68,87</t>
+          <t>R$ 58,33</t>
         </is>
       </c>
       <c r="E78" s="0" t="inlineStr">
         <is>
-          <t>R$ 79,20</t>
+          <t>R$ 67,08</t>
         </is>
       </c>
       <c r="F78" s="0" t="inlineStr">
         <is>
-          <t>741 kcal</t>
+          <t>442 kcal</t>
         </is>
       </c>
       <c r="G78" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H78" s="0" t="inlineStr">
         <is>
@@ -3420,7 +3420,7 @@
       </c>
       <c r="I78" s="0" t="inlineStr">
         <is>
-          <t>23/04/2021</t>
+          <t>28/06/2021</t>
         </is>
       </c>
     </row>
@@ -3440,21 +3440,21 @@
       </c>
       <c r="D79" s="0" t="inlineStr">
         <is>
-          <t>R$ 144,53</t>
+          <t>R$ 75,25</t>
         </is>
       </c>
       <c r="E79" s="0" t="inlineStr">
         <is>
-          <t>R$ 166,21</t>
+          <t>R$ 86,54</t>
         </is>
       </c>
       <c r="F79" s="0" t="inlineStr">
         <is>
-          <t>593 kcal</t>
+          <t>228 kcal</t>
         </is>
       </c>
       <c r="G79" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H79" s="0" t="inlineStr">
         <is>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="I79" s="0" t="inlineStr">
         <is>
-          <t>07/05/2021</t>
+          <t>29/06/2021</t>
         </is>
       </c>
     </row>
@@ -3483,21 +3483,21 @@
       </c>
       <c r="D80" s="0" t="inlineStr">
         <is>
-          <t>R$ 122,14</t>
+          <t>R$ 117,17</t>
         </is>
       </c>
       <c r="E80" s="0" t="inlineStr">
         <is>
-          <t>R$ 140,46</t>
+          <t>R$ 134,75</t>
         </is>
       </c>
       <c r="F80" s="0" t="inlineStr">
         <is>
-          <t>886 kcal</t>
+          <t>489 kcal</t>
         </is>
       </c>
       <c r="G80" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H80" s="0" t="inlineStr">
         <is>
@@ -3506,7 +3506,7 @@
       </c>
       <c r="I80" s="0" t="inlineStr">
         <is>
-          <t>27/04/2021</t>
+          <t>25/06/2021</t>
         </is>
       </c>
     </row>
@@ -3526,21 +3526,21 @@
       </c>
       <c r="D81" s="0" t="inlineStr">
         <is>
-          <t>R$ 129,29</t>
+          <t>R$ 58,70</t>
         </is>
       </c>
       <c r="E81" s="0" t="inlineStr">
         <is>
-          <t>R$ 148,68</t>
+          <t>R$ 67,51</t>
         </is>
       </c>
       <c r="F81" s="0" t="inlineStr">
         <is>
-          <t>747 kcal</t>
+          <t>309 kcal</t>
         </is>
       </c>
       <c r="G81" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H81" s="0" t="inlineStr">
         <is>
@@ -3549,7 +3549,7 @@
       </c>
       <c r="I81" s="0" t="inlineStr">
         <is>
-          <t>03/05/2021</t>
+          <t>01/07/2021</t>
         </is>
       </c>
     </row>
@@ -3569,30 +3569,30 @@
       </c>
       <c r="D82" s="0" t="inlineStr">
         <is>
-          <t>R$ 184,86</t>
+          <t>R$ 150,64</t>
         </is>
       </c>
       <c r="E82" s="0" t="inlineStr">
         <is>
-          <t>R$ 212,59</t>
+          <t>R$ 173,24</t>
         </is>
       </c>
       <c r="F82" s="0" t="inlineStr">
         <is>
-          <t>855 kcal</t>
+          <t>642 kcal</t>
         </is>
       </c>
       <c r="G82" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I82" s="0" t="inlineStr">
         <is>
-          <t>25/04/2021</t>
+          <t>24/06/2021</t>
         </is>
       </c>
     </row>
@@ -3612,21 +3612,21 @@
       </c>
       <c r="D83" s="0" t="inlineStr">
         <is>
-          <t>R$ 155,34</t>
+          <t>R$ 162,73</t>
         </is>
       </c>
       <c r="E83" s="0" t="inlineStr">
         <is>
-          <t>R$ 178,64</t>
+          <t>R$ 187,14</t>
         </is>
       </c>
       <c r="F83" s="0" t="inlineStr">
         <is>
-          <t>701 kcal</t>
+          <t>877 kcal</t>
         </is>
       </c>
       <c r="G83" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H83" s="0" t="inlineStr">
         <is>
@@ -3635,7 +3635,7 @@
       </c>
       <c r="I83" s="0" t="inlineStr">
         <is>
-          <t>30/04/2021</t>
+          <t>29/06/2021</t>
         </is>
       </c>
     </row>
@@ -3655,17 +3655,17 @@
       </c>
       <c r="D84" s="0" t="inlineStr">
         <is>
-          <t>R$ 64,15</t>
+          <t>R$ 132,20</t>
         </is>
       </c>
       <c r="E84" s="0" t="inlineStr">
         <is>
-          <t>R$ 73,77</t>
+          <t>R$ 152,03</t>
         </is>
       </c>
       <c r="F84" s="0" t="inlineStr">
         <is>
-          <t>715 kcal</t>
+          <t>691 kcal</t>
         </is>
       </c>
       <c r="G84" s="0">
@@ -3673,12 +3673,12 @@
       </c>
       <c r="H84" s="0" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="I84" s="0" t="inlineStr">
         <is>
-          <t>12/05/2021</t>
+          <t>26/06/2021</t>
         </is>
       </c>
     </row>
@@ -3698,17 +3698,17 @@
       </c>
       <c r="D85" s="0" t="inlineStr">
         <is>
-          <t>R$ 59,54</t>
+          <t>R$ 195,89</t>
         </is>
       </c>
       <c r="E85" s="0" t="inlineStr">
         <is>
-          <t>R$ 68,47</t>
+          <t>R$ 225,27</t>
         </is>
       </c>
       <c r="F85" s="0" t="inlineStr">
         <is>
-          <t>559 kcal</t>
+          <t>304 kcal</t>
         </is>
       </c>
       <c r="G85" s="0">
@@ -3716,12 +3716,12 @@
       </c>
       <c r="H85" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I85" s="0" t="inlineStr">
         <is>
-          <t>21/05/2021</t>
+          <t>19/06/2021</t>
         </is>
       </c>
     </row>
@@ -3741,17 +3741,17 @@
       </c>
       <c r="D86" s="0" t="inlineStr">
         <is>
-          <t>R$ 187,15</t>
+          <t>R$ 177,39</t>
         </is>
       </c>
       <c r="E86" s="0" t="inlineStr">
         <is>
-          <t>R$ 215,22</t>
+          <t>R$ 204,00</t>
         </is>
       </c>
       <c r="F86" s="0" t="inlineStr">
         <is>
-          <t>857 kcal</t>
+          <t>531 kcal</t>
         </is>
       </c>
       <c r="G86" s="0">
@@ -3759,12 +3759,12 @@
       </c>
       <c r="H86" s="0" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="I86" s="0" t="inlineStr">
         <is>
-          <t>30/04/2021</t>
+          <t>03/07/2021</t>
         </is>
       </c>
     </row>
@@ -3784,30 +3784,30 @@
       </c>
       <c r="D87" s="0" t="inlineStr">
         <is>
-          <t>R$ 56,67</t>
+          <t>R$ 114,73</t>
         </is>
       </c>
       <c r="E87" s="0" t="inlineStr">
         <is>
-          <t>R$ 65,17</t>
+          <t>R$ 131,94</t>
         </is>
       </c>
       <c r="F87" s="0" t="inlineStr">
         <is>
-          <t>871 kcal</t>
+          <t>628 kcal</t>
         </is>
       </c>
       <c r="G87" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H87" s="0" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I87" s="0" t="inlineStr">
         <is>
-          <t>13/05/2021</t>
+          <t>07/07/2021</t>
         </is>
       </c>
     </row>
@@ -3827,30 +3827,30 @@
       </c>
       <c r="D88" s="0" t="inlineStr">
         <is>
-          <t>R$ 66,75</t>
+          <t>R$ 70,91</t>
         </is>
       </c>
       <c r="E88" s="0" t="inlineStr">
         <is>
-          <t>R$ 76,76</t>
+          <t>R$ 81,55</t>
         </is>
       </c>
       <c r="F88" s="0" t="inlineStr">
         <is>
-          <t>778 kcal</t>
+          <t>538 kcal</t>
         </is>
       </c>
       <c r="G88" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H88" s="0" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="I88" s="0" t="inlineStr">
         <is>
-          <t>04/05/2021</t>
+          <t>20/06/2021</t>
         </is>
       </c>
     </row>
@@ -3870,30 +3870,30 @@
       </c>
       <c r="D89" s="0" t="inlineStr">
         <is>
-          <t>R$ 147,91</t>
+          <t>R$ 161,83</t>
         </is>
       </c>
       <c r="E89" s="0" t="inlineStr">
         <is>
-          <t>R$ 170,10</t>
+          <t>R$ 186,10</t>
         </is>
       </c>
       <c r="F89" s="0" t="inlineStr">
         <is>
-          <t>876 kcal</t>
+          <t>771 kcal</t>
         </is>
       </c>
       <c r="G89" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H89" s="0" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="I89" s="0" t="inlineStr">
         <is>
-          <t>19/05/2021</t>
+          <t>09/07/2021</t>
         </is>
       </c>
     </row>
@@ -3913,17 +3913,17 @@
       </c>
       <c r="D90" s="0" t="inlineStr">
         <is>
-          <t>R$ 73,04</t>
+          <t>R$ 76,25</t>
         </is>
       </c>
       <c r="E90" s="0" t="inlineStr">
         <is>
-          <t>R$ 84,00</t>
+          <t>R$ 87,69</t>
         </is>
       </c>
       <c r="F90" s="0" t="inlineStr">
         <is>
-          <t>399 kcal</t>
+          <t>528 kcal</t>
         </is>
       </c>
       <c r="G90" s="0">
@@ -3931,12 +3931,12 @@
       </c>
       <c r="H90" s="0" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I90" s="0" t="inlineStr">
         <is>
-          <t>09/05/2021</t>
+          <t>20/06/2021</t>
         </is>
       </c>
     </row>
@@ -3956,30 +3956,30 @@
       </c>
       <c r="D91" s="0" t="inlineStr">
         <is>
-          <t>R$ 75,34</t>
+          <t>R$ 124,19</t>
         </is>
       </c>
       <c r="E91" s="0" t="inlineStr">
         <is>
-          <t>R$ 86,64</t>
+          <t>R$ 142,82</t>
         </is>
       </c>
       <c r="F91" s="0" t="inlineStr">
         <is>
-          <t>850 kcal</t>
+          <t>190 kcal</t>
         </is>
       </c>
       <c r="G91" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H91" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I91" s="0" t="inlineStr">
         <is>
-          <t>24/04/2021</t>
+          <t>23/06/2021</t>
         </is>
       </c>
     </row>
@@ -3999,30 +3999,30 @@
       </c>
       <c r="D92" s="0" t="inlineStr">
         <is>
-          <t>R$ 153,10</t>
+          <t>R$ 99,25</t>
         </is>
       </c>
       <c r="E92" s="0" t="inlineStr">
         <is>
-          <t>R$ 176,07</t>
+          <t>R$ 114,14</t>
         </is>
       </c>
       <c r="F92" s="0" t="inlineStr">
         <is>
-          <t>808 kcal</t>
+          <t>773 kcal</t>
         </is>
       </c>
       <c r="G92" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H92" s="0" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="I92" s="0" t="inlineStr">
         <is>
-          <t>25/04/2021</t>
+          <t>18/06/2021</t>
         </is>
       </c>
     </row>
@@ -4042,17 +4042,17 @@
       </c>
       <c r="D93" s="0" t="inlineStr">
         <is>
-          <t>R$ 65,25</t>
+          <t>R$ 173,21</t>
         </is>
       </c>
       <c r="E93" s="0" t="inlineStr">
         <is>
-          <t>R$ 75,04</t>
+          <t>R$ 199,19</t>
         </is>
       </c>
       <c r="F93" s="0" t="inlineStr">
         <is>
-          <t>547 kcal</t>
+          <t>736 kcal</t>
         </is>
       </c>
       <c r="G93" s="0">
@@ -4060,12 +4060,12 @@
       </c>
       <c r="H93" s="0" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I93" s="0" t="inlineStr">
         <is>
-          <t>06/05/2021</t>
+          <t>20/06/2021</t>
         </is>
       </c>
     </row>
@@ -4085,30 +4085,30 @@
       </c>
       <c r="D94" s="0" t="inlineStr">
         <is>
-          <t>R$ 74,70</t>
+          <t>R$ 109,92</t>
         </is>
       </c>
       <c r="E94" s="0" t="inlineStr">
         <is>
-          <t>R$ 85,91</t>
+          <t>R$ 126,41</t>
         </is>
       </c>
       <c r="F94" s="0" t="inlineStr">
         <is>
-          <t>284 kcal</t>
+          <t>103 kcal</t>
         </is>
       </c>
       <c r="G94" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H94" s="0" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="I94" s="0" t="inlineStr">
         <is>
-          <t>14/05/2021</t>
+          <t>17/06/2021</t>
         </is>
       </c>
     </row>
@@ -4128,17 +4128,17 @@
       </c>
       <c r="D95" s="0" t="inlineStr">
         <is>
-          <t>R$ 80,11</t>
+          <t>R$ 144,66</t>
         </is>
       </c>
       <c r="E95" s="0" t="inlineStr">
         <is>
-          <t>R$ 92,13</t>
+          <t>R$ 166,36</t>
         </is>
       </c>
       <c r="F95" s="0" t="inlineStr">
         <is>
-          <t>667 kcal</t>
+          <t>508 kcal</t>
         </is>
       </c>
       <c r="G95" s="0">
@@ -4146,12 +4146,12 @@
       </c>
       <c r="H95" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I95" s="0" t="inlineStr">
         <is>
-          <t>07/05/2021</t>
+          <t>19/06/2021</t>
         </is>
       </c>
     </row>
@@ -4171,17 +4171,17 @@
       </c>
       <c r="D96" s="0" t="inlineStr">
         <is>
-          <t>R$ 171,61</t>
+          <t>R$ 67,79</t>
         </is>
       </c>
       <c r="E96" s="0" t="inlineStr">
         <is>
-          <t>R$ 197,35</t>
+          <t>R$ 77,96</t>
         </is>
       </c>
       <c r="F96" s="0" t="inlineStr">
         <is>
-          <t>434 kcal</t>
+          <t>552 kcal</t>
         </is>
       </c>
       <c r="G96" s="0">
@@ -4189,12 +4189,12 @@
       </c>
       <c r="H96" s="0" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I96" s="0" t="inlineStr">
         <is>
-          <t>11/05/2021</t>
+          <t>11/07/2021</t>
         </is>
       </c>
     </row>
@@ -4214,17 +4214,17 @@
       </c>
       <c r="D97" s="0" t="inlineStr">
         <is>
-          <t>R$ 59,48</t>
+          <t>R$ 169,54</t>
         </is>
       </c>
       <c r="E97" s="0" t="inlineStr">
         <is>
-          <t>R$ 68,40</t>
+          <t>R$ 194,97</t>
         </is>
       </c>
       <c r="F97" s="0" t="inlineStr">
         <is>
-          <t>837 kcal</t>
+          <t>613 kcal</t>
         </is>
       </c>
       <c r="G97" s="0">
@@ -4237,7 +4237,7 @@
       </c>
       <c r="I97" s="0" t="inlineStr">
         <is>
-          <t>12/05/2021</t>
+          <t>24/06/2021</t>
         </is>
       </c>
     </row>
@@ -4257,21 +4257,21 @@
       </c>
       <c r="D98" s="0" t="inlineStr">
         <is>
-          <t>R$ 73,64</t>
+          <t>R$ 55,89</t>
         </is>
       </c>
       <c r="E98" s="0" t="inlineStr">
         <is>
-          <t>R$ 84,69</t>
+          <t>R$ 64,27</t>
         </is>
       </c>
       <c r="F98" s="0" t="inlineStr">
         <is>
-          <t>622 kcal</t>
+          <t>328 kcal</t>
         </is>
       </c>
       <c r="G98" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H98" s="0" t="inlineStr">
         <is>
@@ -4280,7 +4280,7 @@
       </c>
       <c r="I98" s="0" t="inlineStr">
         <is>
-          <t>14/05/2021</t>
+          <t>01/07/2021</t>
         </is>
       </c>
     </row>
@@ -4300,30 +4300,30 @@
       </c>
       <c r="D99" s="0" t="inlineStr">
         <is>
-          <t>R$ 140,91</t>
+          <t>R$ 117,33</t>
         </is>
       </c>
       <c r="E99" s="0" t="inlineStr">
         <is>
-          <t>R$ 162,05</t>
+          <t>R$ 134,93</t>
         </is>
       </c>
       <c r="F99" s="0" t="inlineStr">
         <is>
-          <t>114 kcal</t>
+          <t>477 kcal</t>
         </is>
       </c>
       <c r="G99" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H99" s="0" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="I99" s="0" t="inlineStr">
         <is>
-          <t>24/04/2021</t>
+          <t>13/07/2021</t>
         </is>
       </c>
     </row>
@@ -4343,17 +4343,17 @@
       </c>
       <c r="D100" s="0" t="inlineStr">
         <is>
-          <t>R$ 142,27</t>
+          <t>R$ 178,89</t>
         </is>
       </c>
       <c r="E100" s="0" t="inlineStr">
         <is>
-          <t>R$ 163,61</t>
+          <t>R$ 205,72</t>
         </is>
       </c>
       <c r="F100" s="0" t="inlineStr">
         <is>
-          <t>676 kcal</t>
+          <t>887 kcal</t>
         </is>
       </c>
       <c r="G100" s="0">
@@ -4361,12 +4361,12 @@
       </c>
       <c r="H100" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I100" s="0" t="inlineStr">
         <is>
-          <t>25/04/2021</t>
+          <t>17/06/2021</t>
         </is>
       </c>
     </row>
@@ -4386,17 +4386,17 @@
       </c>
       <c r="D101" s="0" t="inlineStr">
         <is>
-          <t>R$ 107,01</t>
+          <t>R$ 193,50</t>
         </is>
       </c>
       <c r="E101" s="0" t="inlineStr">
         <is>
-          <t>R$ 123,06</t>
+          <t>R$ 222,53</t>
         </is>
       </c>
       <c r="F101" s="0" t="inlineStr">
         <is>
-          <t>243 kcal</t>
+          <t>597 kcal</t>
         </is>
       </c>
       <c r="G101" s="0">
@@ -4409,7 +4409,7 @@
       </c>
       <c r="I101" s="0" t="inlineStr">
         <is>
-          <t>19/05/2021</t>
+          <t>29/06/2021</t>
         </is>
       </c>
     </row>
@@ -4429,17 +4429,17 @@
       </c>
       <c r="D102" s="0" t="inlineStr">
         <is>
-          <t>R$ 122,35</t>
+          <t>R$ 132,99</t>
         </is>
       </c>
       <c r="E102" s="0" t="inlineStr">
         <is>
-          <t>R$ 140,70</t>
+          <t>R$ 152,94</t>
         </is>
       </c>
       <c r="F102" s="0" t="inlineStr">
         <is>
-          <t>132 kcal</t>
+          <t>561 kcal</t>
         </is>
       </c>
       <c r="G102" s="0">
@@ -4447,12 +4447,12 @@
       </c>
       <c r="H102" s="0" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="I102" s="0" t="inlineStr">
         <is>
-          <t>09/05/2021</t>
+          <t>03/07/2021</t>
         </is>
       </c>
     </row>
@@ -4472,17 +4472,17 @@
       </c>
       <c r="D103" s="0" t="inlineStr">
         <is>
-          <t>R$ 85,63</t>
+          <t>R$ 163,60</t>
         </is>
       </c>
       <c r="E103" s="0" t="inlineStr">
         <is>
-          <t>R$ 98,47</t>
+          <t>R$ 188,14</t>
         </is>
       </c>
       <c r="F103" s="0" t="inlineStr">
         <is>
-          <t>224 kcal</t>
+          <t>420 kcal</t>
         </is>
       </c>
       <c r="G103" s="0">
@@ -4490,12 +4490,12 @@
       </c>
       <c r="H103" s="0" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="I103" s="0" t="inlineStr">
         <is>
-          <t>27/04/2021</t>
+          <t>04/07/2021</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
upgrade to dev main
</commit_message>
<xml_diff>
--- a/storage/download.xlsx
+++ b/storage/download.xlsx
@@ -205,7 +205,7 @@
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Carne Louca</t>
+          <t>Carne Louca 1</t>
         </is>
       </c>
       <c r="C4" s="0" t="inlineStr">
@@ -315,7 +315,7 @@
         </is>
       </c>
       <c r="G6" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="0" t="inlineStr">
         <is>
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="G11" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="0" t="inlineStr">
         <is>

</xml_diff>